<commit_message>
Search Patient page modified, excel sheet added, case queue page added.
</commit_message>
<xml_diff>
--- a/src/test/resources/Driver/ort_excel.xlsx
+++ b/src/test/resources/Driver/ort_excel.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="NurseData" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="SpdData" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="PatientData" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="SearchPatient" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,42 +23,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t xml:space="preserve">username</t>
-  </si>
-  <si>
-    <t xml:space="preserve">password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Christiana_nurse@mailinator.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ORT@33221</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QANurseOAFacilityOASystemOA@mailinator.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ORT@3322</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lastName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">firstName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dOB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mNR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sharma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vikas</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Christiana_nurse@mailinator.com</t>
+  </si>
+  <si>
+    <t>ORT@33221</t>
+  </si>
+  <si>
+    <t>QANurseOAFacilityOASystemOA@mailinator.com</t>
+  </si>
+  <si>
+    <t>ORT@3322</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>dOB</t>
+  </si>
+  <si>
+    <t>mNR</t>
+  </si>
+  <si>
+    <t>Sharma</t>
+  </si>
+  <si>
+    <t>Vikas</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Date Of Birth (DOB)</t>
+  </si>
+  <si>
+    <t>MNR</t>
+  </si>
+  <si>
+    <t>Specialty</t>
+  </si>
+  <si>
+    <t>Case Number</t>
   </si>
 </sst>
 </file>
@@ -65,9 +84,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -94,6 +113,12 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Courier New"/>
+      <family val="3"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -139,7 +164,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -148,32 +173,37 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="54.59"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.8622448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -207,7 +237,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -216,21 +246,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -239,17 +272,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -279,7 +315,72 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="22.984693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="22.8520408163265"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="2" width="22.984693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="2" width="22.8520408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="2" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>646464</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Updated code after merging with Piyush and Saurabh code
</commit_message>
<xml_diff>
--- a/src/test/resources/Driver/ort_excel.xlsx
+++ b/src/test/resources/Driver/ort_excel.xlsx
@@ -173,10 +173,10 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="A3:C3 A11"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="54.59"/>
   </cols>
@@ -228,10 +228,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A3:C3 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -251,10 +251,10 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:C3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>

</xml_diff>

<commit_message>
Redefined getRowCount() , getColCount() methods. Method to fetch data from cell string and numeric values(working).
</commit_message>
<xml_diff>
--- a/src/test/resources/Driver/ort_excel.xlsx
+++ b/src/test/resources/Driver/ort_excel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="75">
   <si>
     <t>username</t>
   </si>
@@ -74,7 +74,7 @@
     <t>Case Number</t>
   </si>
   <si>
-    <t>Patient DOB</t>
+    <t>Patient DOB (mmddyyy)</t>
   </si>
   <si>
     <t>Specialty</t>
@@ -86,10 +86,46 @@
     <t>John</t>
   </si>
   <si>
+    <t>sports</t>
+  </si>
+  <si>
     <t>Jones</t>
   </si>
   <si>
     <t>Samantha</t>
+  </si>
+  <si>
+    <t>Spine</t>
+  </si>
+  <si>
+    <t>trauma</t>
+  </si>
+  <si>
+    <t>Potter</t>
+  </si>
+  <si>
+    <t>Harry</t>
+  </si>
+  <si>
+    <t>Rock</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Trauma</t>
+  </si>
+  <si>
+    <t>Sports</t>
+  </si>
+  <si>
+    <t>Harper</t>
+  </si>
+  <si>
+    <t>Kelly</t>
+  </si>
+  <si>
+    <t>arthroplasty</t>
   </si>
   <si>
     <t>Module</t>
@@ -393,7 +429,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -416,6 +452,14 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -607,8 +651,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.4336734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.0816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -663,7 +707,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -689,8 +733,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1023" min="1" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1023" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.96428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -731,20 +775,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="3" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="3" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="3" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="3" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -782,6 +827,7 @@
         <v>20</v>
       </c>
       <c r="F2" s="5"/>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -796,14 +842,26 @@
       <c r="D3" s="3" t="n">
         <v>60</v>
       </c>
+      <c r="F3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="F4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
@@ -812,12 +870,107 @@
       <c r="B5" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
       <c r="D6" s="3" t="n">
         <v>20</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>3261996</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>646464</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>10261996</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>646464</v>
+      </c>
+      <c r="D10" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -844,225 +997,226 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="9" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="8" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="6" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="6" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="6" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="6" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="8" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="9" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="9" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="9" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="6" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="6" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="6" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="6" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="6" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="29" min="28" style="6" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="31" min="30" style="6" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="6" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="6" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="1023" min="34" style="6" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="8" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="8" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="10" width="13.5"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="9" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="8" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="8" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="8" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="8" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="8" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="8" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="10" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="11" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="11" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="11" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="8" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="8" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="8" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="8" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="8" width="20.25"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="8" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="29" min="28" style="8" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="31" min="30" style="8" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="8" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="8" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="1023" min="34" style="8" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
-    <row r="1" s="14" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="R1" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="S1" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="T1" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="U1" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="V1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="W1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="X1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="AD1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="AF1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="AG1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="AMJ1" s="15"/>
+    <row r="1" s="16" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="S1" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="T1" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="U1" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="V1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="W1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="X1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AG1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AMJ1" s="17"/>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="K2" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q2" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="R2" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="S2" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="T2" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="U2" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="V2" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="W2" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="X2" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y2" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z2" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA2" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB2" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC2" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD2" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE2" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="AF2" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG2" s="16" t="s">
-        <v>32</v>
+      <c r="A2" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q2" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="S2" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="T2" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="U2" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="V2" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="W2" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="X2" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y2" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z2" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA2" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB2" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC2" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD2" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE2" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF2" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG2" s="18" t="s">
+        <v>44</v>
       </c>
       <c r="AH2" s="0"/>
       <c r="AI2" s="0"/>
@@ -2055,103 +2209,103 @@
       <c r="AMH2" s="0"/>
       <c r="AMI2" s="0"/>
     </row>
-    <row r="3" s="29" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="I3" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="J3" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="K3" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="L3" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="M3" s="24" t="s">
+    <row r="3" s="31" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="N3" s="24" t="s">
+      <c r="B3" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="O3" s="24" t="s">
+      <c r="C3" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="P3" s="24" t="s">
+      <c r="D3" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="Q3" s="24" t="s">
+      <c r="E3" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="R3" s="26" t="s">
+      <c r="F3" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="S3" s="27" t="s">
+      <c r="G3" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="T3" s="27" t="s">
+      <c r="H3" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="U3" s="27" t="s">
+      <c r="I3" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="V3" s="24" t="s">
+      <c r="J3" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="W3" s="24" t="s">
+      <c r="K3" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="X3" s="24" t="s">
+      <c r="L3" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="Y3" s="24" t="s">
+      <c r="M3" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="Z3" s="24" t="s">
+      <c r="N3" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="AA3" s="24" t="s">
+      <c r="O3" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="AB3" s="24" t="s">
+      <c r="P3" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="AC3" s="24" t="s">
+      <c r="Q3" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="AD3" s="28"/>
-      <c r="AE3" s="28"/>
-      <c r="AF3" s="28"/>
-      <c r="AG3" s="28"/>
-      <c r="AMJ3" s="30"/>
+      <c r="R3" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="S3" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="T3" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="U3" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="V3" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="W3" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="X3" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y3" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z3" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA3" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB3" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC3" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD3" s="30"/>
+      <c r="AE3" s="30"/>
+      <c r="AF3" s="30"/>
+      <c r="AG3" s="30"/>
+      <c r="AMJ3" s="32"/>
     </row>
     <row r="4" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="31" t="s">
-        <v>62</v>
+      <c r="A4" s="33" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. Search Patient using Excel sheet (specific Patient) - Complete.  2. ExcelDataUtility specific method to fetch string values and numeric values - Complete.  3. Dynamic method to Search Pateint (pass sheet name, row, column information as parameters during test case creation) - Complete
</commit_message>
<xml_diff>
--- a/src/test/resources/Driver/ort_excel.xlsx
+++ b/src/test/resources/Driver/ort_excel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="74">
   <si>
     <t>username</t>
   </si>
@@ -80,13 +80,7 @@
     <t>Specialty</t>
   </si>
   <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>sports</t>
+    <t>Trauma</t>
   </si>
   <si>
     <t>Jones</t>
@@ -113,9 +107,6 @@
     <t>James</t>
   </si>
   <si>
-    <t>Trauma</t>
-  </si>
-  <si>
     <t>Sports</t>
   </si>
   <si>
@@ -126,6 +117,12 @@
   </si>
   <si>
     <t>arthroplasty</t>
+  </si>
+  <si>
+    <t>Keller</t>
+  </si>
+  <si>
+    <t>Sam</t>
   </si>
   <si>
     <t>Module</t>
@@ -289,13 +286,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="10"/>
       <name val="Courier New"/>
       <family val="3"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
       <sz val="10"/>
       <name val="Courier New"/>
       <family val="3"/>
@@ -442,27 +439,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -494,7 +491,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -554,7 +551,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -562,7 +559,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -646,13 +643,13 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.0816326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -707,7 +704,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -728,13 +725,13 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1023" min="1" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1023" min="1" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.83163265306122"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -775,21 +772,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="3" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="3" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="3" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="1023" min="8" style="3" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -826,42 +824,51 @@
       <c r="D2" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6"/>
+      <c r="E2" s="6" t="n">
+        <v>3261996</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>646464</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="E3" s="6" t="n">
+        <v>3261996</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="3" t="n">
-        <v>505152</v>
-      </c>
-      <c r="D3" s="3" t="n">
-        <v>60</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5" t="n">
+        <v>646464</v>
+      </c>
+      <c r="D4" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="G3" s="6"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="3" t="n">
-        <v>20</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="6"/>
+      <c r="E4" s="6" t="n">
+        <v>3261996</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
@@ -870,107 +877,725 @@
       <c r="B5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="G5" s="6"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="E5" s="6" t="n">
+        <v>3261996</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="3" t="n">
+      <c r="A6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>646464</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6" t="n">
+        <v>3261996</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>646464</v>
+      </c>
+      <c r="D7" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="E6" s="3" t="n">
+      <c r="E7" s="6"/>
+      <c r="F7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="5" t="n">
+        <v>646464</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="E8" s="6" t="n">
         <v>3261996</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F8" s="6"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6"/>
+      <c r="B10" s="0"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="0"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="6"/>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="0"/>
+      <c r="D12" s="0"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0"/>
+      <c r="B13" s="0"/>
+      <c r="C13" s="0"/>
+      <c r="D13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0"/>
+      <c r="B14" s="0"/>
+      <c r="C14" s="0"/>
+      <c r="D14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="0"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="6" t="n">
+        <v>20</v>
+      </c>
+      <c r="E16" s="0"/>
+      <c r="F16" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="0"/>
+      <c r="F17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="6" t="n">
+        <v>20</v>
+      </c>
+      <c r="E18" s="6" t="n">
+        <v>3261996</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="C19" s="6" t="n">
+        <v>123456</v>
+      </c>
+      <c r="D19" s="0"/>
+      <c r="E19" s="0"/>
+      <c r="F19" s="0"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B20" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="3" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+      <c r="C20" s="6" t="n">
+        <v>123789</v>
+      </c>
+      <c r="D20" s="0"/>
+      <c r="E20" s="0"/>
+      <c r="F20" s="0"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="6" t="n">
+        <v>646464</v>
+      </c>
+      <c r="D21" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="E21" s="6" t="n">
+        <v>10261996</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="0"/>
+      <c r="C22" s="6" t="n">
+        <v>646464</v>
+      </c>
+      <c r="D22" s="0"/>
+      <c r="E22" s="6" t="n">
+        <v>5272021</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="6" t="n">
+        <v>20</v>
+      </c>
+      <c r="F23" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="3" t="s">
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+      <c r="B24" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="0"/>
+      <c r="D24" s="0"/>
+      <c r="F24" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0"/>
+      <c r="B25" s="0"/>
+      <c r="C25" s="0"/>
+      <c r="D25" s="0"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0"/>
+      <c r="B26" s="0"/>
+      <c r="C26" s="0"/>
+      <c r="D26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B27" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="3" t="n">
-        <v>646464</v>
-      </c>
-      <c r="D9" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="E9" s="3" t="n">
-        <v>10261996</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="3" t="n">
-        <v>646464</v>
-      </c>
-      <c r="D10" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="3" t="n">
+      <c r="C27" s="0"/>
+      <c r="D27" s="0"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0"/>
+      <c r="B28" s="0"/>
+      <c r="C28" s="0"/>
+      <c r="D28" s="0"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0"/>
+      <c r="B29" s="0"/>
+      <c r="C29" s="0"/>
+      <c r="D29" s="0"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0"/>
+      <c r="B30" s="0"/>
+      <c r="C30" s="0"/>
+      <c r="D30" s="0"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0"/>
+      <c r="B31" s="0"/>
+      <c r="C31" s="0"/>
+      <c r="D31" s="0"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0"/>
+      <c r="B32" s="0"/>
+      <c r="C32" s="0"/>
+      <c r="D32" s="0"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0"/>
+      <c r="B33" s="0"/>
+      <c r="C33" s="0"/>
+      <c r="D33" s="0"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0"/>
+      <c r="B34" s="0"/>
+      <c r="C34" s="0"/>
+      <c r="D34" s="0"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0"/>
+      <c r="B35" s="0"/>
+      <c r="C35" s="0"/>
+      <c r="D35" s="0"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0"/>
+      <c r="B36" s="0"/>
+      <c r="C36" s="0"/>
+      <c r="D36" s="0"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0"/>
+      <c r="B37" s="0"/>
+      <c r="C37" s="0"/>
+      <c r="D37" s="0"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0"/>
+      <c r="B38" s="0"/>
+      <c r="C38" s="0"/>
+      <c r="D38" s="0"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0"/>
+      <c r="B39" s="0"/>
+      <c r="C39" s="0"/>
+      <c r="D39" s="0"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0"/>
+      <c r="B40" s="0"/>
+      <c r="C40" s="0"/>
+      <c r="D40" s="0"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0"/>
+      <c r="B41" s="0"/>
+      <c r="C41" s="0"/>
+      <c r="D41" s="0"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0"/>
+      <c r="B42" s="0"/>
+      <c r="C42" s="0"/>
+      <c r="D42" s="0"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0"/>
+      <c r="B43" s="0"/>
+      <c r="C43" s="0"/>
+      <c r="D43" s="0"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0"/>
+      <c r="B44" s="0"/>
+      <c r="C44" s="0"/>
+      <c r="D44" s="0"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0"/>
+      <c r="B45" s="0"/>
+      <c r="C45" s="0"/>
+      <c r="D45" s="0"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0"/>
+      <c r="B46" s="0"/>
+      <c r="C46" s="0"/>
+      <c r="D46" s="0"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0"/>
+      <c r="B47" s="0"/>
+      <c r="C47" s="0"/>
+      <c r="D47" s="0"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0"/>
+      <c r="B48" s="0"/>
+      <c r="C48" s="0"/>
+      <c r="D48" s="0"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0"/>
+      <c r="B49" s="0"/>
+      <c r="C49" s="0"/>
+      <c r="D49" s="0"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0"/>
+      <c r="B50" s="0"/>
+      <c r="C50" s="0"/>
+      <c r="D50" s="0"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0"/>
+      <c r="B51" s="0"/>
+      <c r="C51" s="0"/>
+      <c r="D51" s="0"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0"/>
+      <c r="B52" s="0"/>
+      <c r="C52" s="0"/>
+      <c r="D52" s="0"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0"/>
+      <c r="B53" s="0"/>
+      <c r="C53" s="0"/>
+      <c r="D53" s="0"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0"/>
+      <c r="B54" s="0"/>
+      <c r="C54" s="0"/>
+      <c r="D54" s="0"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0"/>
+      <c r="B55" s="0"/>
+      <c r="C55" s="0"/>
+      <c r="D55" s="0"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0"/>
+      <c r="B56" s="0"/>
+      <c r="C56" s="0"/>
+      <c r="D56" s="0"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0"/>
+      <c r="B57" s="0"/>
+      <c r="C57" s="0"/>
+      <c r="D57" s="0"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0"/>
+      <c r="B58" s="0"/>
+      <c r="C58" s="0"/>
+      <c r="D58" s="0"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0"/>
+      <c r="B59" s="0"/>
+      <c r="C59" s="0"/>
+      <c r="D59" s="0"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0"/>
+      <c r="B60" s="0"/>
+      <c r="C60" s="0"/>
+      <c r="D60" s="0"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0"/>
+      <c r="B61" s="0"/>
+      <c r="C61" s="0"/>
+      <c r="D61" s="0"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0"/>
+      <c r="B62" s="0"/>
+      <c r="C62" s="0"/>
+      <c r="D62" s="0"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0"/>
+      <c r="B63" s="0"/>
+      <c r="C63" s="0"/>
+      <c r="D63" s="0"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0"/>
+      <c r="B64" s="0"/>
+      <c r="C64" s="0"/>
+      <c r="D64" s="0"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0"/>
+      <c r="B65" s="0"/>
+      <c r="C65" s="0"/>
+      <c r="D65" s="0"/>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0"/>
+      <c r="B66" s="0"/>
+      <c r="C66" s="0"/>
+      <c r="D66" s="0"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0"/>
+      <c r="B67" s="0"/>
+      <c r="C67" s="0"/>
+      <c r="D67" s="0"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0"/>
+      <c r="B68" s="0"/>
+      <c r="C68" s="0"/>
+      <c r="D68" s="0"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0"/>
+      <c r="B69" s="0"/>
+      <c r="C69" s="0"/>
+      <c r="D69" s="0"/>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0"/>
+      <c r="B70" s="0"/>
+      <c r="C70" s="0"/>
+      <c r="D70" s="0"/>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0"/>
+      <c r="B71" s="0"/>
+      <c r="C71" s="0"/>
+      <c r="D71" s="0"/>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0"/>
+      <c r="B72" s="0"/>
+      <c r="C72" s="0"/>
+      <c r="D72" s="0"/>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0"/>
+      <c r="B73" s="0"/>
+      <c r="C73" s="0"/>
+      <c r="D73" s="0"/>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0"/>
+      <c r="B74" s="0"/>
+      <c r="C74" s="0"/>
+      <c r="D74" s="0"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0"/>
+      <c r="B75" s="0"/>
+      <c r="C75" s="0"/>
+      <c r="D75" s="0"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0"/>
+      <c r="B76" s="0"/>
+      <c r="C76" s="0"/>
+      <c r="D76" s="0"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0"/>
+      <c r="B77" s="0"/>
+      <c r="C77" s="0"/>
+      <c r="D77" s="0"/>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0"/>
+      <c r="B78" s="0"/>
+      <c r="C78" s="0"/>
+      <c r="D78" s="0"/>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0"/>
+      <c r="B79" s="0"/>
+      <c r="C79" s="0"/>
+      <c r="D79" s="0"/>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0"/>
+      <c r="B80" s="0"/>
+      <c r="C80" s="0"/>
+      <c r="D80" s="0"/>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0"/>
+      <c r="B81" s="0"/>
+      <c r="C81" s="0"/>
+      <c r="D81" s="0"/>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0"/>
+      <c r="B82" s="0"/>
+      <c r="C82" s="0"/>
+      <c r="D82" s="0"/>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0"/>
+      <c r="B83" s="0"/>
+      <c r="C83" s="0"/>
+      <c r="D83" s="0"/>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0"/>
+      <c r="B84" s="0"/>
+      <c r="C84" s="0"/>
+      <c r="D84" s="0"/>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0"/>
+      <c r="B85" s="0"/>
+      <c r="C85" s="0"/>
+      <c r="D85" s="0"/>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0"/>
+      <c r="B86" s="0"/>
+      <c r="C86" s="0"/>
+      <c r="D86" s="0"/>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0"/>
+      <c r="B87" s="0"/>
+      <c r="C87" s="0"/>
+      <c r="D87" s="0"/>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0"/>
+      <c r="B88" s="0"/>
+      <c r="C88" s="0"/>
+      <c r="D88" s="0"/>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0"/>
+      <c r="B89" s="0"/>
+      <c r="C89" s="0"/>
+      <c r="D89" s="0"/>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0"/>
+      <c r="B90" s="0"/>
+      <c r="C90" s="0"/>
+      <c r="D90" s="0"/>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0"/>
+      <c r="B91" s="0"/>
+      <c r="C91" s="0"/>
+      <c r="D91" s="0"/>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0"/>
+      <c r="B92" s="0"/>
+      <c r="C92" s="0"/>
+      <c r="D92" s="0"/>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0"/>
+      <c r="B93" s="0"/>
+      <c r="C93" s="0"/>
+      <c r="D93" s="0"/>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0"/>
+      <c r="B94" s="0"/>
+      <c r="C94" s="0"/>
+      <c r="D94" s="0"/>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0"/>
+      <c r="B95" s="0"/>
+      <c r="C95" s="0"/>
+      <c r="D95" s="0"/>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0"/>
+      <c r="B96" s="0"/>
+      <c r="C96" s="0"/>
+      <c r="D96" s="0"/>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0"/>
+      <c r="B97" s="0"/>
+      <c r="C97" s="0"/>
+      <c r="D97" s="0"/>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0"/>
+      <c r="B98" s="0"/>
+      <c r="C98" s="0"/>
+      <c r="D98" s="0"/>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0"/>
+      <c r="B99" s="0"/>
+      <c r="C99" s="0"/>
+      <c r="D99" s="0"/>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C100" s="6" t="n">
+        <v>9560</v>
+      </c>
+      <c r="D100" s="6" t="n">
         <v>20</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -997,144 +1622,144 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="8" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="8" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="10" width="13.5"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="9" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="8" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="8" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="8" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="8" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="8" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="8" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="10" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="11" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="11" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="11" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="8" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="8" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="8" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="8" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="8" width="20.25"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="8" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="29" min="28" style="8" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="31" min="30" style="8" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="8" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="8" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="1023" min="34" style="8" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="13.5"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="10" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="9" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="3" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="3" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="3" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="3" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="3" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="3" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="10" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="11" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="11" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="11" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="3" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="3" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="3" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="3" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="3" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="3" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="29" min="28" style="3" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="31" min="30" style="3" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="3" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="3" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="1023" min="34" style="3" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="16" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="15" t="s">
+      <c r="E1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="L1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>38</v>
-      </c>
       <c r="M1" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O1" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q1" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R1" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S1" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T1" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U1" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="V1" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="W1" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X1" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y1" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Z1" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AA1" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AB1" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AC1" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AD1" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AE1" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AF1" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AG1" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AMJ1" s="17"/>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="19"/>
       <c r="C2" s="20"/>
@@ -1144,79 +1769,79 @@
       <c r="G2" s="22"/>
       <c r="H2" s="20"/>
       <c r="I2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="P2" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q2" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="R2" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="S2" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="J2" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="K2" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="L2" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="M2" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="N2" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="O2" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="P2" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q2" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="R2" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="S2" s="25" t="s">
+      <c r="T2" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="T2" s="25" t="s">
+      <c r="U2" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="U2" s="25" t="s">
+      <c r="V2" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="V2" s="18" t="s">
-        <v>44</v>
-      </c>
       <c r="W2" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="X2" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Y2" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Z2" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AA2" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AB2" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AC2" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AD2" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AE2" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AF2" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AG2" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AH2" s="0"/>
       <c r="AI2" s="0"/>
@@ -2211,91 +2836,91 @@
     </row>
     <row r="3" s="31" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="C3" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="D3" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="E3" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="F3" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="G3" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="H3" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="28" t="s">
+      <c r="I3" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="I3" s="27" t="s">
+      <c r="J3" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="K3" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="K3" s="26" t="s">
+      <c r="L3" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="L3" s="26" t="s">
+      <c r="M3" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="M3" s="26" t="s">
+      <c r="N3" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="N3" s="26" t="s">
+      <c r="O3" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="O3" s="26" t="s">
+      <c r="P3" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="P3" s="26" t="s">
+      <c r="Q3" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="Q3" s="26" t="s">
+      <c r="R3" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="R3" s="28" t="s">
+      <c r="S3" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="S3" s="29" t="s">
+      <c r="T3" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="T3" s="29" t="s">
+      <c r="U3" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="U3" s="29" t="s">
+      <c r="V3" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="V3" s="26" t="s">
+      <c r="W3" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="W3" s="26" t="s">
+      <c r="X3" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="X3" s="26" t="s">
+      <c r="Y3" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="Y3" s="26" t="s">
+      <c r="Z3" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="Z3" s="26" t="s">
+      <c r="AA3" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="AA3" s="26" t="s">
+      <c r="AB3" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="AB3" s="26" t="s">
+      <c r="AC3" s="26" t="s">
         <v>72</v>
-      </c>
-      <c r="AC3" s="26" t="s">
-        <v>73</v>
       </c>
       <c r="AD3" s="30"/>
       <c r="AE3" s="30"/>
@@ -2305,7 +2930,7 @@
     </row>
     <row r="4" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SearchPatientPage - Added popup repository, Added - SPDInProgressTest, SPDOnHoldTest. Modified - CaseQueueTest.
</commit_message>
<xml_diff>
--- a/src/test/resources/Driver/ort_excel.xlsx
+++ b/src/test/resources/Driver/ort_excel.xlsx
@@ -74,10 +74,10 @@
     <t>Case Number</t>
   </si>
   <si>
-    <t>Patient DOB (mmddyyy)</t>
-  </si>
-  <si>
-    <t>Specialty</t>
+    <t>Patient DOB (mmddyyyy)</t>
+  </si>
+  <si>
+    <t>Specialty (Spine, Arthroplasty, Trauma, Sports)</t>
   </si>
   <si>
     <t>Trauma</t>
@@ -648,8 +648,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.5408163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.4642857142857"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -703,9 +702,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.2602040816327"/>
-  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -730,8 +726,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1023" min="1" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.56122448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -775,19 +770,18 @@
   <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="3" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="1023" min="8" style="3" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="3" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="26.5102040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="58.2551020408163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="1023" min="8" style="3" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -940,9 +934,7 @@
       <c r="D8" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="E8" s="6" t="n">
-        <v>3261996</v>
-      </c>
+      <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="8"/>
     </row>
@@ -950,7 +942,9 @@
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
+      <c r="D9" s="6" t="n">
+        <v>20</v>
+      </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
@@ -966,27 +960,39 @@
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="7"/>
-      <c r="D11" s="6"/>
+      <c r="D11" s="6" t="n">
+        <v>330</v>
+      </c>
+      <c r="E11" s="0"/>
       <c r="F11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="0"/>
-      <c r="D12" s="0"/>
+      <c r="D12" s="6" t="n">
+        <v>308</v>
+      </c>
+      <c r="E12" s="0"/>
       <c r="F12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0"/>
       <c r="B13" s="0"/>
       <c r="C13" s="0"/>
-      <c r="D13" s="0"/>
+      <c r="D13" s="6" t="n">
+        <v>310</v>
+      </c>
+      <c r="E13" s="0"/>
+      <c r="F13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0"/>
       <c r="B14" s="0"/>
       <c r="C14" s="0"/>
       <c r="D14" s="0"/>
+      <c r="E14" s="0"/>
+      <c r="F14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6"/>
@@ -1622,37 +1628,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="13.5"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="10" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="9" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="3" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="3" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="3" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="3" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="3" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="3" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="10" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="11" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="11" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="11" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="3" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="3" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="3" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="3" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="3" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="3" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="29" min="28" style="3" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="31" min="30" style="3" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="3" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="3" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="1023" min="34" style="3" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="10" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="9" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="3" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="3" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="3" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="3" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="3" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="10" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="11" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="11" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="11" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="3" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="3" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="3" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="3" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="3" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="3" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="29" min="28" style="3" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="31" min="30" style="3" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="3" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="3" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="1023" min="34" style="3" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.96428571428571"/>
   </cols>
   <sheetData>
     <row r="1" s="16" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Removed unneccesary class files
</commit_message>
<xml_diff>
--- a/src/test/resources/Driver/ort_excel.xlsx
+++ b/src/test/resources/Driver/ort_excel.xlsx
@@ -176,7 +176,7 @@
       <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="54.59"/>
   </cols>
@@ -231,7 +231,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -254,7 +254,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>

</xml_diff>

<commit_message>
Updated Code with Dataprovider Excel
</commit_message>
<xml_diff>
--- a/src/test/resources/Driver/ort_excel.xlsx
+++ b/src/test/resources/Driver/ort_excel.xlsx
@@ -14,6 +14,7 @@
     <sheet name="SearchPatient" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="CreateCaseLongFlow" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="LongFlow" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Sheet7" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="93">
   <si>
     <t xml:space="preserve">username</t>
   </si>
@@ -295,6 +296,15 @@
   </si>
   <si>
     <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Active</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inactive</t>
   </si>
 </sst>
 </file>
@@ -3030,7 +3040,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3182,4 +3192,134 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="53.21"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="36" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added modified procedure selection flow
</commit_message>
<xml_diff>
--- a/src/test/resources/Driver/ort_excel.xlsx
+++ b/src/test/resources/Driver/ort_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="NurseData" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="104">
   <si>
     <t xml:space="preserve">username</t>
   </si>
@@ -336,6 +336,9 @@
   </si>
   <si>
     <t xml:space="preserve">IM Nail Hip / InterTroch / CMN Hip (27245)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ExFix Distal Femur/ Exfix Femoral Shaft(20692+27500)</t>
   </si>
 </sst>
 </file>
@@ -754,7 +757,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.3359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="54.59"/>
   </cols>
@@ -809,7 +812,7 @@
       <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.3359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="13" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="2" t="s">
@@ -852,7 +855,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.3359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
@@ -1755,7 +1758,7 @@
       <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
@@ -3247,11 +3250,11 @@
   </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
@@ -3414,11 +3417,11 @@
   </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
@@ -3426,7 +3429,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="50.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="52.8"/>
   </cols>
   <sheetData>
@@ -3505,7 +3508,7 @@
         <v>23</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="I3" s="11"/>
     </row>

</xml_diff>

<commit_message>
Updated Procedure Selection Page
</commit_message>
<xml_diff>
--- a/src/test/resources/Driver/ort_excel.xlsx
+++ b/src/test/resources/Driver/ort_excel.xlsx
@@ -754,10 +754,10 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="I1:I3 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.40625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="54.59"/>
   </cols>
@@ -809,10 +809,10 @@
   <dimension ref="B13:D15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="1" sqref="I1:I3 D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.40625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="13" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="2" t="s">
@@ -852,10 +852,10 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="I1:I3 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.40625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
@@ -901,7 +901,7 @@
   <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="1" sqref="I1:I3 D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1755,10 +1755,10 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="1" sqref="I1:I3 H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
@@ -1917,7 +1917,7 @@
   <dimension ref="A1:AMJ4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="I1:I3 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3250,11 +3250,11 @@
   </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="I1:I3 B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
@@ -3417,11 +3417,11 @@
   </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1:I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>

</xml_diff>

<commit_message>
Added Creat Cart Functionality Code
</commit_message>
<xml_diff>
--- a/src/test/resources/Driver/ort_excel.xlsx
+++ b/src/test/resources/Driver/ort_excel.xlsx
@@ -836,7 +836,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="54.59"/>
   </cols>
@@ -891,7 +891,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
@@ -1790,11 +1790,11 @@
   </sheetPr>
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M13" activeCellId="0" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.30859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.31640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
@@ -3383,7 +3383,7 @@
       <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.30859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.31640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
@@ -3550,7 +3550,7 @@
       <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.30859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.31640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
@@ -3717,7 +3717,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.34"/>
@@ -3790,7 +3790,7 @@
       <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.53"/>

</xml_diff>

<commit_message>
Modified Search Case Flow Page
</commit_message>
<xml_diff>
--- a/src/test/resources/Driver/ort_excel.xlsx
+++ b/src/test/resources/Driver/ort_excel.xlsx
@@ -5,18 +5,19 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="NurseData" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="PatientData" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="SearchPatient" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="LongFlow" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="CreateCaseLongFlow" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="PreferenceCardSelectionFlow" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="ProcedureSelectionFlow" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="LoginUsers" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="SearchCaseFlow" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="SearchCaseFlow2" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="NurseData" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="PatientData" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="SearchPatient" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="LongFlow" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="CreateCaseLongFlow" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="PreferenceCardSelectionFlow" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="ProcedureSelectionFlow" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="LoginUsers" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="SearchCaseFlow" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -28,7 +29,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="134">
+  <si>
+    <t xml:space="preserve">lastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MRN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">speciality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">caseNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sharma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vikas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trauma</t>
+  </si>
   <si>
     <t xml:space="preserve">username</t>
   </si>
@@ -48,12 +73,6 @@
     <t xml:space="preserve">ORT@3322</t>
   </si>
   <si>
-    <t xml:space="preserve">lastName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">firstName</t>
-  </si>
-  <si>
     <t xml:space="preserve">mNR</t>
   </si>
   <si>
@@ -84,9 +103,6 @@
     <t xml:space="preserve">Specialty (Spine, Arthroplasty, Trauma, Sports)</t>
   </si>
   <si>
-    <t xml:space="preserve">Trauma</t>
-  </si>
-  <si>
     <t xml:space="preserve">Jones</t>
   </si>
   <si>
@@ -141,9 +157,6 @@
     <t xml:space="preserve">patientAllergy</t>
   </si>
   <si>
-    <t xml:space="preserve">speciality</t>
-  </si>
-  <si>
     <t xml:space="preserve">notesBySurgeon</t>
   </si>
   <si>
@@ -417,16 +430,7 @@
     <t xml:space="preserve">christiana_hcp@mailinator.com</t>
   </si>
   <si>
-    <t xml:space="preserve">MRN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">caseNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sharma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vikas</t>
+    <t xml:space="preserve">ORT@54321</t>
   </si>
 </sst>
 </file>
@@ -839,39 +843,286 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44.87"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>646464</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>646464</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>646464</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="29.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="44.87"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>646464</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>646464</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>646464</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="ORT@54321"/>
+    <hyperlink ref="C3" r:id="rId2" display="ORT@54321"/>
+    <hyperlink ref="C4" r:id="rId3" display="ORT@54321"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="54.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -889,7 +1140,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -900,31 +1151,31 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -938,7 +1189,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -963,31 +1214,31 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C2" s="5" t="n">
         <v>646464</v>
@@ -999,14 +1250,14 @@
         <v>3261996</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="G2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5"/>
       <c r="B3" s="5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C3" s="5" t="n">
         <v>646464</v>
@@ -1018,13 +1269,13 @@
         <v>3261996</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="G3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5" t="n">
@@ -1037,16 +1288,16 @@
         <v>3261996</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="G4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="n">
@@ -1056,16 +1307,16 @@
         <v>3261996</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="G5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>646464</v>
@@ -1075,16 +1326,16 @@
         <v>3261996</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="G6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C7" s="5" t="n">
         <v>646464</v>
@@ -1094,16 +1345,16 @@
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="G7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C8" s="5" t="n">
         <v>646464</v>
@@ -1181,10 +1432,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="6" t="n">
@@ -1192,15 +1443,15 @@
       </c>
       <c r="E16" s="0"/>
       <c r="F16" s="6" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -1218,15 +1469,15 @@
         <v>3261996</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C19" s="6" t="n">
         <v>123456</v>
@@ -1237,10 +1488,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C20" s="6" t="n">
         <v>123789</v>
@@ -1251,10 +1502,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C21" s="6" t="n">
         <v>646464</v>
@@ -1266,12 +1517,12 @@
         <v>10261996</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B22" s="0"/>
       <c r="C22" s="6" t="n">
@@ -1282,35 +1533,35 @@
         <v>5272021</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="6" t="n">
         <v>20</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C24" s="0"/>
       <c r="D24" s="0"/>
       <c r="F24" s="6" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1327,10 +1578,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C27" s="0"/>
       <c r="D27" s="0"/>
@@ -1769,10 +2020,10 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="6" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C100" s="6" t="n">
         <v>9560</v>
@@ -1792,18 +2043,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.43359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.31"/>
@@ -1818,237 +2069,237 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F3" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="N3" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="G3" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="J3" s="0" t="s">
+      <c r="O3" s="0" t="s">
         <v>59</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="M3" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="N3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="O3" s="0" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" s="10" t="s">
+      <c r="G4" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="N4" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="M4" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="N4" s="0" t="s">
-        <v>54</v>
-      </c>
       <c r="O4" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2062,7 +2313,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2109,109 +2360,109 @@
   <sheetData>
     <row r="1" s="19" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="L1" s="15" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="M1" s="15" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="N1" s="15" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="O1" s="15" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="P1" s="15" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="Q1" s="15" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="R1" s="17" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="S1" s="18" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="T1" s="18" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="U1" s="18" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="V1" s="15" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="W1" s="15" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="X1" s="15" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="Y1" s="15" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="Z1" s="15" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="AA1" s="15" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="AB1" s="15" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="AC1" s="15" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="AD1" s="15" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="AE1" s="15" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="AF1" s="15" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="AG1" s="15" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="AMJ1" s="20"/>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="21" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B2" s="22"/>
       <c r="C2" s="23"/>
@@ -2221,79 +2472,79 @@
       <c r="G2" s="25"/>
       <c r="H2" s="23"/>
       <c r="I2" s="26" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="L2" s="21" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="M2" s="21" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="N2" s="21" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="O2" s="21" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="P2" s="21" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="Q2" s="21" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="R2" s="27" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="S2" s="28" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="T2" s="28" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="U2" s="28" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="V2" s="21" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="W2" s="21" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="X2" s="21" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="Y2" s="21" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="Z2" s="21" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AA2" s="21" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AB2" s="21" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AC2" s="21" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AD2" s="21" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AE2" s="21" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AF2" s="21" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AG2" s="21" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AH2" s="0"/>
       <c r="AI2" s="0"/>
@@ -3288,91 +3539,91 @@
     </row>
     <row r="3" s="34" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="H3" s="31" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="I3" s="30" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="J3" s="29" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="K3" s="29" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="L3" s="29" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="M3" s="29" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="N3" s="29" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="O3" s="29" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="P3" s="29" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="Q3" s="29" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="R3" s="31" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="S3" s="32" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="T3" s="32" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="U3" s="32" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="V3" s="29" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="W3" s="29" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="X3" s="29" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="Y3" s="29" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="Z3" s="29" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="AA3" s="29" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="AB3" s="29" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="AC3" s="29" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="AD3" s="33"/>
       <c r="AE3" s="33"/>
@@ -3382,190 +3633,8 @@
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="36" t="s">
-        <v>110</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:J5"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.43359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="52.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="52.8"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="0" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="J3" s="11"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="J4" s="11"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="J5" s="11"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3586,166 +3655,166 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.43359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="21.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="50.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="52.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="52.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>46</v>
+        <v>117</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>58</v>
-      </c>
       <c r="G4" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="J4" s="11"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="J5" s="11"/>
     </row>
@@ -3765,62 +3834,171 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="47.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="21.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="50.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="52.8"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>123</v>
+        <v>38</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="0" t="s">
         <v>124</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>126</v>
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>127</v>
+        <v>60</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="0" t="s">
         <v>126</v>
       </c>
+      <c r="J3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>128</v>
+        <v>49</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>3</v>
+        <v>66</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>126</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="J4" s="11"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="J5" s="11"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3838,128 +4016,64 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="47.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="0" t="s">
         <v>129</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>646464</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>510</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>131</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>646464</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>20</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>132</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>646464</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>54</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="ORT@33221"/>
-    <hyperlink ref="B4" r:id="rId2" display="ORT@33221"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
modified preference card Method
</commit_message>
<xml_diff>
--- a/src/test/resources/Driver/ort_excel.xlsx
+++ b/src/test/resources/Driver/ort_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="SearchCaseFlow2" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="144">
   <si>
     <t xml:space="preserve">lastName</t>
   </si>
@@ -178,42 +178,42 @@
     <t xml:space="preserve">Instructions</t>
   </si>
   <si>
+    <t xml:space="preserve">Active</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christiana surgeon </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Critical (Up to 1hr.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do not drink water one hour before Surgery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Local</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bilateral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bleach Chair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Instructions</t>
+  </si>
+  <si>
     <t xml:space="preserve">Inactive</t>
   </si>
   <si>
-    <t xml:space="preserve">Christiana surgeon </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Critical (Up to 1hr.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do not drink water one hour before Surgery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Local</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bilateral</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bleach Chair</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No Comments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No Instructions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Active</t>
-  </si>
-  <si>
     <t xml:space="preserve">V</t>
   </si>
   <si>
@@ -376,10 +376,31 @@
     <t xml:space="preserve">Test Data (TC_001)</t>
   </si>
   <si>
-    <t xml:space="preserve">surgeonName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preferenceCard</t>
+    <t xml:space="preserve">SurgeonName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UrgencyName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PatientAllergy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speciality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PhysicianAssistant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NotesBySurgeon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PreferenceCardSelection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AnesthesiaRequest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Positions</t>
   </si>
   <si>
     <t xml:space="preserve">Michael J. Principe </t>
@@ -388,6 +409,12 @@
     <t xml:space="preserve">ARTHRODESIS (FUSION) ANKLE W/WO GRAFT</t>
   </si>
   <si>
+    <t xml:space="preserve">Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beach Chair</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nicholas Quercetti </t>
   </si>
   <si>
@@ -401,6 +428,9 @@
   </si>
   <si>
     <t xml:space="preserve">IM Nail Hip / InterTroch / CMN Hip(27245)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A</t>
   </si>
   <si>
     <t xml:space="preserve">procedureSelection</t>
@@ -849,11 +879,11 @@
       <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.28"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -946,7 +976,7 @@
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="29.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.53"/>
@@ -958,13 +988,13 @@
         <v>38</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>0</v>
@@ -984,16 +1014,16 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>5</v>
@@ -1013,16 +1043,16 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>5</v>
@@ -1042,16 +1072,16 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>5</v>
@@ -1096,7 +1126,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="54.59"/>
   </cols>
@@ -1151,7 +1181,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
@@ -2050,11 +2080,11 @@
   </sheetPr>
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.31"/>
@@ -2210,7 +2240,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>66</v>
@@ -2257,7 +2287,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>15</v>
@@ -3652,13 +3682,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="19.31"/>
@@ -3666,8 +3696,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="52.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="52.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="31.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="53.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="22.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.98"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3681,27 +3714,51 @@
         <v>1</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>14</v>
+        <v>91</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>115</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>41</v>
+        <v>117</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>3</v>
+        <v>118</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>15</v>
@@ -3713,7 +3770,7 @@
         <v>17</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>51</v>
@@ -3725,12 +3782,36 @@
         <v>7</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>118</v>
+        <v>72</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>15</v>
@@ -3742,7 +3823,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>62</v>
@@ -3754,13 +3835,36 @@
         <v>7</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="J3" s="11"/>
+        <v>52</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>15</v>
@@ -3772,7 +3876,7 @@
         <v>17</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>62</v>
@@ -3784,13 +3888,36 @@
         <v>7</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="J4" s="11"/>
+        <v>72</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q4" s="0" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>15</v>
@@ -3814,9 +3941,32 @@
         <v>7</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="J5" s="11"/>
+        <v>52</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q5" s="0" t="s">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3840,7 +3990,7 @@
       <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.31"/>
@@ -3878,12 +4028,12 @@
         <v>3</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>15</v>
@@ -3907,12 +4057,12 @@
         <v>7</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>15</v>
@@ -3936,13 +4086,13 @@
         <v>7</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="J3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>66</v>
@@ -3966,13 +4116,13 @@
         <v>7</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="J4" s="11"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>15</v>
@@ -3996,7 +4146,7 @@
         <v>7</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="J5" s="11"/>
     </row>
@@ -4022,7 +4172,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.34"/>
@@ -4031,13 +4181,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4048,29 +4198,29 @@
         <v>11</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Create Case Flow Page
</commit_message>
<xml_diff>
--- a/src/test/resources/Driver/ort_excel.xlsx
+++ b/src/test/resources/Driver/ort_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="SearchCaseFlow2" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="144">
   <si>
     <t xml:space="preserve">lastName</t>
   </si>
@@ -879,7 +879,7 @@
       <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.53"/>
@@ -976,7 +976,7 @@
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="29.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.53"/>
@@ -1126,7 +1126,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.90234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="54.59"/>
   </cols>
@@ -1181,7 +1181,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.90234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
@@ -2080,11 +2080,11 @@
   </sheetPr>
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.31"/>
@@ -2350,8 +2350,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3684,11 +3684,11 @@
   </sheetPr>
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T18" activeCellId="0" sqref="T18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="19.31"/>
@@ -3984,13 +3984,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.31"/>
@@ -4000,6 +4000,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="50.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="52.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="20.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4030,10 +4031,28 @@
       <c r="I1" s="0" t="s">
         <v>134</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>15</v>
@@ -4059,10 +4078,28 @@
       <c r="I2" s="0" t="s">
         <v>135</v>
       </c>
+      <c r="J2" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>15</v>
@@ -4088,7 +4125,24 @@
       <c r="I3" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="J3" s="11"/>
+      <c r="J3" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -4118,7 +4172,24 @@
       <c r="I4" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="J4" s="11"/>
+      <c r="J4" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -4148,7 +4219,24 @@
       <c r="I5" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="J5" s="11"/>
+      <c r="J5" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4166,60 +4254,72 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="47.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="32.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="47.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>140</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added search cases and open cases TestCases
</commit_message>
<xml_diff>
--- a/src/test/resources/Driver/ort_excel.xlsx
+++ b/src/test/resources/Driver/ort_excel.xlsx
@@ -5,19 +5,19 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
-    <sheet name="SearchCaseFlow2" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="NurseData" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="PatientData" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="SearchPatient" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="LongFlow" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="CreateCaseLongFlow" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="PreferenceCardSelectionFlow" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="ProcedureSelectionFlow" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="LoginUsers" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="SearchCaseFlow" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="NurseData" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="PatientData" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="SearchPatient" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="LongFlow" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="CreateCaseLongFlow" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="PreferenceCardSelectionFlow" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="ProcedureSelectionFlow" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="LoginUsers" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="SearchCaseFlow" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="OpenCases" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -29,7 +29,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="152">
+  <si>
+    <t xml:space="preserve">username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christiana_nurse@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORT@33221</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QANurseOAFacilityOASystemOA@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORT@3322</t>
+  </si>
   <si>
     <t xml:space="preserve">lastName</t>
   </si>
@@ -37,12 +55,417 @@
     <t xml:space="preserve">firstName</t>
   </si>
   <si>
+    <t xml:space="preserve">mNR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sharma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vikas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">646464</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient Last Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient First Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient MNR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Case Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient DOB (mmddyyyy)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specialty (Spine, Arthroplasty, Trauma, Sports)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trauma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samantha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trauma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">James</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sports</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kelly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arthroplasty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">urgencyName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">patientAllergy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">speciality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notesBySurgeon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AnasthesiaRequest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Side</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PositioningComments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instructions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Active</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christiana surgeon </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Critical (Up to 1hr.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do not drink water one hour before Surgery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Local</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bilateral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bleach Chair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Instructions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inactive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normal (Up to 48hrs.) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A/C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christiana hcp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christiana 44_Test </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Urgent (Up to 8hrs.) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select Facility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find Patient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Case </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub-Module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basic Details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Affected Area </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Procedure Selection </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Selection </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set Selection </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Field / Option</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facility Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MNR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surgeon </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surgeon Allergy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Second Surgeon </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Second Surgeon Allergy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient Allergy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Physician Assistant </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Urgency </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speciality </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surgery Date and Time </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Body Part </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Procedure </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anesthesia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Block Anesthesia Type </t>
+  </si>
+  <si>
+    <t xml:space="preserve">X Ray </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medication </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Side </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Position </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Position Comment </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instructions </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Data (TC_001)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SurgeonName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UrgencyName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PatientAllergy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speciality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PhysicianAssistant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NotesBySurgeon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PreferenceCardSelection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AnesthesiaRequest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Positions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michael J. Principe </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARTHRODESIS (FUSION) ANKLE W/WO GRAFT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beach Chair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nicholas Quercetti </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IM HIP STRYKER GAMMA NAIL      (INTRAMEDULLARY)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eric T. Johnson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXTERNAL FIXATOR SMALL APPLICATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IM Nail Hip / InterTroch / CMN Hip(27245)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">procedureSelection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OpenQuantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IM Nail Hip / InterTroch / CMN Hip (27245)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,2,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ExFix Distal Femur/ Exfix Femoral Shaft(20692+27500)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,2,2,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,3,2,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,4,3,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">userRoleLoginId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">userRolePassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">facilitySelection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wilmington, DE, 19899 , Wilmington, Delaware, 19899</t>
+  </si>
+  <si>
+    <t xml:space="preserve">christiana_spd@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">christiana_hcp@mailinator.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">MRN</t>
   </si>
   <si>
-    <t xml:space="preserve">speciality</t>
-  </si>
-  <si>
     <t xml:space="preserve">caseNumber</t>
   </si>
   <si>
@@ -52,430 +475,16 @@
     <t xml:space="preserve">vikas</t>
   </si>
   <si>
-    <t xml:space="preserve">Trauma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">username</t>
-  </si>
-  <si>
-    <t xml:space="preserve">password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Christiana_nurse@mailinator.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ORT@33221</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QANurseOAFacilityOASystemOA@mailinator.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ORT@3322</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mNR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sharma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vikas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">646464</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patient Last Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patient First Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patient MNR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Case Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patient DOB (mmddyyyy)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Specialty (Spine, Arthroplasty, Trauma, Sports)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Samantha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">trauma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Potter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Harry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">James</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sports</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Harper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kelly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">arthroplasty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">urgencyName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">patientAllergy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">notesBySurgeon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AnasthesiaRequest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medications</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Side</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Position</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PositioningComments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Instructions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Active</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Christiana surgeon </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Critical (Up to 1hr.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do not drink water one hour before Surgery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Local</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bilateral</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bleach Chair</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No Comments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No Instructions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inactive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Normal (Up to 48hrs.) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">A/C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Right</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Christiana hcp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Christiana 44_Test </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Urgent (Up to 8hrs.) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">General</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Module</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Login</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Select Facility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Find Patient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create Case </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sub-Module</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basic Details</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Affected Area </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Procedure Selection </t>
-  </si>
-  <si>
-    <t xml:space="preserve">System Selection </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Set Selection </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Field / Option</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Facility Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Last Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MNR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DOB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surgeon </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surgeon Allergy </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Second Surgeon </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Second Surgeon Allergy </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patient Allergy </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Physician Assistant </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Urgency </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Speciality </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surgery Date and Time </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Body Part </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Procedure </t>
-  </si>
-  <si>
-    <t xml:space="preserve">System </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anesthesia </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Block Anesthesia Type </t>
-  </si>
-  <si>
-    <t xml:space="preserve">X Ray </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medication </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Side </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Position </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Position Comment </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Instructions </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Data (TC_001)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SurgeonName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UrgencyName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PatientAllergy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Speciality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PhysicianAssistant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotesBySurgeon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PreferenceCardSelection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AnesthesiaRequest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Positions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Michael J. Principe </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARTHRODESIS (FUSION) ANKLE W/WO GRAFT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Left</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beach Chair</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nicholas Quercetti </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IM HIP STRYKER GAMMA NAIL      (INTRAMEDULLARY)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eric T. Johnson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXTERNAL FIXATOR SMALL APPLICATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IM Nail Hip / InterTroch / CMN Hip(27245)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N/A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">procedureSelection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OpenQuantity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IM Nail Hip / InterTroch / CMN Hip (27245)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ExFix Distal Femur/ Exfix Femoral Shaft(20692+27500)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,2,2,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,3,2,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,4,3,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">userRoleLoginId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">userRolePassword</t>
-  </si>
-  <si>
-    <t xml:space="preserve">facilitySelection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wilmington, DE, 19899 , Wilmington, Delaware, 19899</t>
-  </si>
-  <si>
-    <t xml:space="preserve">christiana_spd@mailinator.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">christiana_hcp@mailinator.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ORT@54321</t>
+    <t xml:space="preserve">LastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FirstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vikash</t>
   </si>
 </sst>
 </file>
@@ -888,17 +897,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="54.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -908,71 +915,31 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="B3" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>646464</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>646464</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>646464</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>54</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="ORT@33221"/>
+    <hyperlink ref="A3" r:id="rId2" display="QANurseOAFacilityOASystemOA@mailinator.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -985,141 +952,55 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="29.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="44.87"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>144</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>4</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>145</v>
+        <v>9</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>646464</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>646464</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>646464</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>646464</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>54</v>
+        <v>18</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="ORT@54321"/>
-    <hyperlink ref="C3" r:id="rId2" display="ORT@54321"/>
-    <hyperlink ref="C4" r:id="rId3" display="ORT@54321"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1135,92 +1016,37 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="54.59"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="ORT@33221"/>
-    <hyperlink ref="A3" r:id="rId2" display="QANurseOAFacilityOASystemOA@mailinator.com"/>
-  </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1234,7 +1060,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1259,31 +1085,31 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C2" s="5" t="n">
         <v>646464</v>
@@ -1295,14 +1121,14 @@
         <v>3261996</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="G2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5"/>
       <c r="B3" s="5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C3" s="5" t="n">
         <v>646464</v>
@@ -1314,13 +1140,13 @@
         <v>3261996</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="G3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5" t="n">
@@ -1333,16 +1159,16 @@
         <v>3261996</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="G4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="n">
@@ -1352,16 +1178,16 @@
         <v>3261996</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="G5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>646464</v>
@@ -1371,16 +1197,16 @@
         <v>3261996</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="G6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C7" s="5" t="n">
         <v>646464</v>
@@ -1390,16 +1216,16 @@
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="G7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C8" s="5" t="n">
         <v>646464</v>
@@ -1477,10 +1303,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="6" t="n">
@@ -1488,15 +1314,15 @@
       </c>
       <c r="E16" s="0"/>
       <c r="F16" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -1514,15 +1340,15 @@
         <v>3261996</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C19" s="6" t="n">
         <v>123456</v>
@@ -1533,10 +1359,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C20" s="6" t="n">
         <v>123789</v>
@@ -1547,10 +1373,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C21" s="6" t="n">
         <v>646464</v>
@@ -1562,12 +1388,12 @@
         <v>10261996</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B22" s="0"/>
       <c r="C22" s="6" t="n">
@@ -1578,35 +1404,35 @@
         <v>5272021</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="6" t="n">
         <v>20</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C24" s="0"/>
       <c r="D24" s="0"/>
       <c r="F24" s="6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1623,10 +1449,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C27" s="0"/>
       <c r="D27" s="0"/>
@@ -2065,10 +1891,10 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C100" s="6" t="n">
         <v>9560</v>
@@ -2088,7 +1914,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2096,10 +1922,10 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.31"/>
@@ -2114,237 +1940,237 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="9" t="s">
+      <c r="J1" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="K1" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="L1" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="0" t="s">
+      <c r="M1" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="N1" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="O1" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="10" t="s">
+      <c r="J2" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="K2" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="L2" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="0" t="s">
+      <c r="M2" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="N2" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="O2" s="0" t="s">
         <v>55</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="O2" s="0" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L3" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="0" t="s">
+      <c r="M3" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="K3" s="0" t="s">
+      <c r="N3" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="O3" s="0" t="s">
         <v>55</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="M3" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="N3" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="O3" s="0" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G4" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="K4" s="0" t="s">
+      <c r="M4" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="O4" s="0" t="s">
         <v>55</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="M4" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="N4" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="O4" s="0" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="11" t="s">
+      <c r="J5" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="M5" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="J5" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="K5" s="0" t="s">
+      <c r="N5" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="O5" s="0" t="s">
         <v>55</v>
-      </c>
-      <c r="L5" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="M5" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="N5" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="O5" s="0" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2358,7 +2184,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2405,109 +2231,109 @@
   <sheetData>
     <row r="1" s="19" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>78</v>
-      </c>
       <c r="J1" s="15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="L1" s="15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M1" s="15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="N1" s="15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="O1" s="15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="P1" s="15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="Q1" s="15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="R1" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="S1" s="18" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="T1" s="18" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="U1" s="18" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="V1" s="15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="W1" s="15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="X1" s="15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="Y1" s="15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="Z1" s="15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AA1" s="15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AB1" s="15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AC1" s="15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AD1" s="15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AE1" s="15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AF1" s="15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AG1" s="15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AMJ1" s="20"/>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="21" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B2" s="22"/>
       <c r="C2" s="23"/>
@@ -2517,79 +2343,79 @@
       <c r="G2" s="25"/>
       <c r="H2" s="23"/>
       <c r="I2" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="O2" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="P2" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q2" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="R2" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="S2" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="T2" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="U2" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="V2" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="W2" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="X2" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="Y2" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="Z2" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="N2" s="21" t="s">
+      <c r="AA2" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="O2" s="21" t="s">
+      <c r="AB2" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="P2" s="21" t="s">
+      <c r="AC2" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="Q2" s="21" t="s">
+      <c r="AD2" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="R2" s="27" t="s">
+      <c r="AE2" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="S2" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="T2" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="U2" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="V2" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="W2" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="X2" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="Y2" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="Z2" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="AA2" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="AB2" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="AC2" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="AD2" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="AE2" s="21" t="s">
-        <v>84</v>
-      </c>
       <c r="AF2" s="21" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="AG2" s="21" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="AH2" s="0"/>
       <c r="AI2" s="0"/>
@@ -3584,91 +3410,91 @@
     </row>
     <row r="3" s="34" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="F3" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="G3" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="H3" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="I3" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="J3" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="K3" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="H3" s="31" t="s">
+      <c r="L3" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="I3" s="30" t="s">
+      <c r="M3" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="J3" s="29" t="s">
+      <c r="N3" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="K3" s="29" t="s">
+      <c r="O3" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="L3" s="29" t="s">
+      <c r="P3" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="M3" s="29" t="s">
+      <c r="Q3" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="N3" s="29" t="s">
+      <c r="R3" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="O3" s="29" t="s">
+      <c r="S3" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="P3" s="29" t="s">
+      <c r="T3" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="Q3" s="29" t="s">
+      <c r="U3" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="R3" s="31" t="s">
+      <c r="V3" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="S3" s="32" t="s">
+      <c r="W3" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="T3" s="32" t="s">
+      <c r="X3" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="U3" s="32" t="s">
+      <c r="Y3" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="V3" s="29" t="s">
+      <c r="Z3" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="W3" s="29" t="s">
+      <c r="AA3" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="X3" s="29" t="s">
+      <c r="AB3" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="Y3" s="29" t="s">
+      <c r="AC3" s="29" t="s">
         <v>109</v>
-      </c>
-      <c r="Z3" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="AA3" s="29" t="s">
-        <v>111</v>
-      </c>
-      <c r="AB3" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="AC3" s="29" t="s">
-        <v>113</v>
       </c>
       <c r="AD3" s="33"/>
       <c r="AE3" s="33"/>
@@ -3678,7 +3504,309 @@
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="36" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:Q5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T18" activeCellId="0" sqref="T18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="31.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="53.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="22.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.98"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="H1" s="0" t="s">
         <v>114</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q4" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q5" s="0" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -3697,290 +3825,273 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T18" activeCellId="0" sqref="T18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="21.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="31.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="53.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="22.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="50.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="24.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="20.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>91</v>
+        <v>8</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>115</v>
+        <v>34</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>116</v>
+        <v>35</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>117</v>
+        <v>36</v>
       </c>
       <c r="H1" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="K1" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="L1" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="J1" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="M1" s="0" t="s">
+      <c r="O1" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="P1" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="P1" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q1" s="0" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>124</v>
+        <v>46</v>
       </c>
       <c r="F2" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>73</v>
-      </c>
       <c r="M2" s="0" t="s">
-        <v>55</v>
+        <v>122</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>127</v>
+        <v>51</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q2" s="0" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="0" t="s">
+      <c r="N3" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="M3" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="N3" s="0" t="s">
-        <v>64</v>
-      </c>
       <c r="O3" s="0" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q3" s="0" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>15</v>
+        <v>62</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>130</v>
+        <v>63</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>72</v>
+        <v>128</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>72</v>
+        <v>136</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>131</v>
+        <v>64</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>55</v>
+        <v>122</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>126</v>
+        <v>65</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q4" s="0" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="M5" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="L5" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="M5" s="0" t="s">
-        <v>55</v>
-      </c>
       <c r="N5" s="0" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="P5" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q5" s="0" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -3999,273 +4110,73 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="21.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="50.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="24.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="20.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="32.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="47.37"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>0</v>
+        <v>138</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>1</v>
+        <v>139</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="P1" s="0" t="s">
-        <v>48</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="O2" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="P2" s="0" t="s">
-        <v>55</v>
+        <v>3</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>15</v>
+        <v>142</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="M3" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="N3" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="O3" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="P3" s="0" t="s">
-        <v>55</v>
+        <v>3</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>66</v>
+        <v>143</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="M4" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="N4" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="O4" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="P4" s="0" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="J5" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>141</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="L5" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="M5" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="N5" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="O5" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="P5" s="0" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -4284,76 +4195,141 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="32.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="47.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="29.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="44.87"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>144</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>11</v>
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>145</v>
+        <v>141</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>646464</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>510</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>145</v>
+      <c r="F3" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>646464</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>145</v>
+      <c r="G4" s="0" t="n">
+        <v>646464</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="ORT@33221"/>
+    <hyperlink ref="C3" r:id="rId2" display="ORT@33221"/>
+    <hyperlink ref="C4" r:id="rId3" display="ORT@33221"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
added cart review page
</commit_message>
<xml_diff>
--- a/src/test/resources/Driver/ort_excel.xlsx
+++ b/src/test/resources/Driver/ort_excel.xlsx
@@ -903,7 +903,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="54.59"/>
   </cols>
@@ -955,10 +955,10 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1008,7 +1008,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>151</v>
+        <v>57</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>646464</v>
@@ -1042,7 +1042,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
@@ -1945,7 +1945,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.31"/>
@@ -3549,7 +3549,7 @@
       <selection pane="topLeft" activeCell="T18" activeCellId="0" sqref="T18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="19.31"/>
@@ -3851,7 +3851,7 @@
       <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.31"/>
@@ -4136,7 +4136,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="32.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.34"/>
@@ -4221,7 +4221,7 @@
       <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="29.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.53"/>

</xml_diff>

<commit_message>
Modified Search case and Open Case Pages
</commit_message>
<xml_diff>
--- a/src/test/resources/Driver/ort_excel.xlsx
+++ b/src/test/resources/Driver/ort_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="NurseData" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="153">
   <si>
     <t xml:space="preserve">username</t>
   </si>
@@ -467,6 +467,9 @@
   </si>
   <si>
     <t xml:space="preserve">caseNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORT@54321</t>
   </si>
   <si>
     <t xml:space="preserve">sharma</t>
@@ -903,7 +906,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.19140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="54.59"/>
   </cols>
@@ -954,21 +957,21 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>33</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>144</v>
@@ -977,7 +980,7 @@
         <v>114</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -988,7 +991,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>646464</v>
@@ -997,7 +1000,7 @@
         <v>18</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>619</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -1022,7 +1025,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.19140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
@@ -1925,7 +1928,7 @@
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.31"/>
@@ -3529,7 +3532,7 @@
       <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="19.31"/>
@@ -3831,7 +3834,7 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.31"/>
@@ -4116,7 +4119,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.23828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="32.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.34"/>
@@ -4197,11 +4200,11 @@
   </sheetPr>
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="29.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.53"/>
@@ -4245,16 +4248,16 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>146</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>141</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>646464</v>
@@ -4280,10 +4283,10 @@
         <v>141</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>646464</v>
@@ -4297,7 +4300,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>143</v>
@@ -4309,10 +4312,10 @@
         <v>141</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>646464</v>
@@ -4326,7 +4329,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="ORT@33221"/>
+    <hyperlink ref="C2" r:id="rId1" display="ORT@54321"/>
     <hyperlink ref="C3" r:id="rId2" display="ORT@33221"/>
     <hyperlink ref="C4" r:id="rId3" display="ORT@33221"/>
   </hyperlinks>

</xml_diff>